<commit_message>
few corrections after change history review
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_itemshape_2/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_itemshape_2/WG_Number_excel_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="-4360" yWindow="-20060" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG_Number_excel_table" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
   <si>
     <t>ISO 10303-1023 ed3 part_view_definition Document</t>
   </si>
@@ -104,18 +104,6 @@
     <t>ISO 10303-1712 ed4 part_feature_function ARM EXPRESS</t>
   </si>
   <si>
-    <t>ISO 10303-1717 ed3 part_template_3d_shape Document</t>
-  </si>
-  <si>
-    <t>ISO 10303-1717 ed3 part_template_3d_shape ARM EXPRESS</t>
-  </si>
-  <si>
-    <t>ISO 10303-1722 ed2 part_template Document</t>
-  </si>
-  <si>
-    <t>ISO 10303-1722 ed2 part_template ARM EXPRESS</t>
-  </si>
-  <si>
     <t>ISO 10303-1796 ed2 kinematic_motion_representation Document</t>
   </si>
   <si>
@@ -306,13 +294,31 @@
   </si>
   <si>
     <t>N9373</t>
+  </si>
+  <si>
+    <t>CANCELLED ISO 10303-1717 ed3 part_template_3d_shape ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1717 ed4 part_template_3d_shape Document</t>
+  </si>
+  <si>
+    <t>Changed from ed3 to ed4</t>
+  </si>
+  <si>
+    <t>ISO 10303-1722 ed4 part_template Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1722 ed4 part_template ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>Changed from ed2 to ed4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,6 +335,22 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -376,8 +398,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -391,7 +415,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -667,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,20 +706,21 @@
     <col min="3" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="89.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="24.5" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1">
         <v>42705</v>
@@ -701,15 +728,15 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1">
         <v>42705</v>
@@ -717,15 +744,15 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1">
         <v>42705</v>
@@ -733,15 +760,15 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1">
         <v>42705</v>
@@ -749,10 +776,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -765,10 +792,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -781,10 +808,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -797,10 +824,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -813,10 +840,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -829,10 +856,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -845,10 +872,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -861,10 +888,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -877,10 +904,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -893,10 +920,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -909,10 +936,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -925,10 +952,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -939,12 +966,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -955,12 +982,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -971,12 +998,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -987,12 +1014,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1003,12 +1030,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1019,12 +1046,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1035,12 +1062,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1051,12 +1078,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1067,12 +1094,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1083,12 +1110,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1099,12 +1126,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1115,12 +1142,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1131,12 +1158,12 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1147,273 +1174,277 @@
         <v>42705</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="F30" s="1">
         <v>42705</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="G30" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="1">
-        <v>42705</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="F32" s="1">
         <v>42705</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="F33" s="1">
         <v>42705</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F34" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F35" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F36" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F37" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F38" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F39" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F40" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F41" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F42" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F43" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F44" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F45" s="1">
         <v>42705</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F46" s="1">
         <v>42705</v>

</xml_diff>